<commit_message>
added atkinson and KnightBodnar functions
</commit_message>
<xml_diff>
--- a/data-raw/FIdata.xlsx
+++ b/data-raw/FIdata.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Fiid</t>
   </si>
@@ -30,19 +30,7 @@
     <t>Tmice</t>
   </si>
   <si>
-    <t>DD01_01_01</t>
-  </si>
-  <si>
-    <t>DD01_01_02</t>
-  </si>
-  <si>
-    <t>DD01_01_03</t>
-  </si>
-  <si>
-    <t>DD01_02_01</t>
-  </si>
-  <si>
-    <t>DD01_02_02</t>
+    <t>NaK_ratio</t>
   </si>
 </sst>
 </file>
@@ -360,15 +348,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -378,60 +366,316 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2">
-        <v>-12</v>
+        <v>-1</v>
       </c>
       <c r="C2">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>-14</v>
+        <v>-2</v>
       </c>
       <c r="C3">
         <v>109</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>-12</v>
+        <v>-3</v>
       </c>
       <c r="C4">
         <v>110</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="C5">
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>-5</v>
+      </c>
+      <c r="C6">
+        <v>120</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>-6</v>
+      </c>
+      <c r="C7">
+        <v>90</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B6">
-        <v>-4</v>
-      </c>
-      <c r="C6">
+      <c r="B8">
+        <v>-7</v>
+      </c>
+      <c r="C8">
+        <v>85</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>-8</v>
+      </c>
+      <c r="C9">
+        <v>105</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>-9</v>
+      </c>
+      <c r="C10">
+        <v>125</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>-10</v>
+      </c>
+      <c r="C11">
+        <v>140</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>-11</v>
+      </c>
+      <c r="C12">
+        <v>195</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>-12</v>
+      </c>
+      <c r="C13">
+        <v>165</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>-13</v>
+      </c>
+      <c r="C14">
+        <v>140</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>-14</v>
+      </c>
+      <c r="C15">
+        <v>98</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>-15</v>
+      </c>
+      <c r="C16">
+        <v>160</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>-16</v>
+      </c>
+      <c r="C17">
+        <v>85</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>-17</v>
+      </c>
+      <c r="C18">
+        <v>142</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>-18</v>
+      </c>
+      <c r="C19">
+        <v>180</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>-19</v>
+      </c>
+      <c r="C20">
         <v>75</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>-20</v>
+      </c>
+      <c r="C21">
+        <v>68</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>-21</v>
+      </c>
+      <c r="C22">
+        <v>91</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>-22</v>
+      </c>
+      <c r="C23">
+        <v>75</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>